<commit_message>
Adicionando novos dados de clima na planilha
</commit_message>
<xml_diff>
--- a/DadosClima/clima.xlsx
+++ b/DadosClima/clima.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -702,6 +702,33 @@
         </is>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>São Paulo</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>26/08/2025 21:05</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Nublado</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Adicionando o código do projeto e a planilha
</commit_message>
<xml_diff>
--- a/DadosClima/clima.xlsx
+++ b/DadosClima/clima.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -429,7 +429,7 @@
     <col width="18" customWidth="1" min="2" max="2"/>
     <col width="11" customWidth="1" min="3" max="3"/>
     <col width="13" customWidth="1" min="4" max="4"/>
-    <col width="22" customWidth="1" min="5" max="5"/>
+    <col width="29" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -729,6 +729,357 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>São Paulo</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>26/08/2025 21:49</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Nublado</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>São Paulo</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>26/08/2025 22:22</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Nublado</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>São Paulo</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>26/08/2025 23:22</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>91</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Nublado</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>São Paulo</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>26/08/2025 23:25</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>92</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Nublado</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>São Paulo</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>26/08/2025 23:27</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>92</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Nublado</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>São Paulo</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>26/08/2025 23:58</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>94</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Nublado</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>São Paulo</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>27/08/2025 00:02</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>94</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Nublado</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>BRASILIA</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>27/08/2025 00:03</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Céu limpo com poucas nuvens</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>BARSILIA</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>27/08/2025 00:05</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Céu limpo com poucas nuvens</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>BARSILIA</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>27/08/2025 00:06</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Céu limpo com poucas nuvens</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>BARSILIA</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>27/08/2025 00:07</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Céu limpo com poucas nuvens</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>São Paulo</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>27/08/2025 00:10</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>94</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Nublado</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>São Paulo</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>27/08/2025 00:25</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>94</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Nublado</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>